<commit_message>
Fixed AC simulation.  Schematic now ready.
</commit_message>
<xml_diff>
--- a/Power Supplies/Trim Temp Variation/Power Supply Trimming.xlsx
+++ b/Power Supplies/Trim Temp Variation/Power Supply Trimming.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eric\Z SAMD21 Bare Metal\Power Supplies\Trim Temp Variation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C23FE24-1CFA-4C62-9EFB-7921C237840B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DADA613-2173-419C-9D91-47385AD4C379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1710" yWindow="-120" windowWidth="27210" windowHeight="16440" xr2:uid="{DD6541E9-83B4-470B-BCB9-FFD7587ABBED}"/>
+    <workbookView xWindow="1728" yWindow="-108" windowWidth="21420" windowHeight="14616" xr2:uid="{DD6541E9-83B4-470B-BCB9-FFD7587ABBED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>R</t>
   </si>
@@ -85,6 +85,48 @@
   </si>
   <si>
     <t>ADR4533BRZ</t>
+  </si>
+  <si>
+    <t>LM4132CQ1MFT3.3</t>
+  </si>
+  <si>
+    <t>ADR366BUJZ</t>
+  </si>
+  <si>
+    <t>Temp Coef</t>
+  </si>
+  <si>
+    <t>Noise</t>
+  </si>
+  <si>
+    <t>±0.13%</t>
+  </si>
+  <si>
+    <t>9ppm/°C</t>
+  </si>
+  <si>
+    <t>9.3µVp-p</t>
+  </si>
+  <si>
+    <t>±0.2%</t>
+  </si>
+  <si>
+    <t>20ppm/°C</t>
+  </si>
+  <si>
+    <t>310µVp-p</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>2.1µVp-p</t>
+  </si>
+  <si>
+    <t>2ppm/°C</t>
+  </si>
+  <si>
+    <t>±0.02%</t>
   </si>
 </sst>
 </file>
@@ -457,56 +499,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B7F62D-E556-47EF-88E0-8C5EDB50C261}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A2:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="9.140625" style="1"/>
-    <col min="9" max="9" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="1"/>
+    <col min="7" max="7" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>-40</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
@@ -518,7 +561,7 @@
         <v>0.96772499999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>0.01</v>
       </c>
@@ -530,7 +573,7 @@
         <v>1.0327249999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -550,7 +593,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>1E-4</v>
       </c>
@@ -572,7 +615,7 @@
         <v>397.88744050786988</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -586,7 +629,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <f>A11-A9*A11</f>
         <v>9.9000000000000008E-5</v>
@@ -604,7 +647,7 @@
         <v>-0.1065075000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -618,7 +661,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <f>A11+A9*A11</f>
         <v>1.01E-4</v>
@@ -634,6 +677,71 @@
       <c r="D15" s="4">
         <f>C15-C11</f>
         <v>0.10799249999999994</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="1">
+        <v>10.8</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="1">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="1">
+        <v>4.24</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>